<commit_message>
ENH: reset text fields in queryDBWin
</commit_message>
<xml_diff>
--- a/featuresChecklist.xlsx
+++ b/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,11 @@
           <t>modelmodel</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>676</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -460,6 +465,9 @@
       <c r="D2" t="n">
         <v>1</v>
       </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -505,6 +513,9 @@
       <c r="E5" t="n">
         <v>1</v>
       </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -533,6 +544,9 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ENH: added documentation + removed init files
</commit_message>
<xml_diff>
--- a/featuresChecklist.xlsx
+++ b/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,11 @@
           <t>676</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>56Model</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,6 +486,9 @@
       <c r="D3" t="n">
         <v>1</v>
       </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -497,6 +505,9 @@
       <c r="D4" t="n">
         <v>1</v>
       </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -514,6 +525,9 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DEPLOY: resetting needed files
</commit_message>
<xml_diff>
--- a/featuresChecklist.xlsx
+++ b/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,36 +432,6 @@
           <t>defaultModel</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>new2</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>modelmodel</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>676</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>56Model</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -472,15 +442,6 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -491,15 +452,6 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -510,18 +462,6 @@
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -532,21 +472,6 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -557,9 +482,6 @@
       <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -570,9 +492,6 @@
       <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="H7" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -583,12 +502,6 @@
       <c r="B8" t="n">
         <v>1</v>
       </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -599,9 +512,6 @@
       <c r="B9" t="n">
         <v>1</v>
       </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -612,9 +522,6 @@
       <c r="B10" t="n">
         <v>1</v>
       </c>
-      <c r="H10" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -623,9 +530,6 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>